<commit_message>
rename sentiment txt file & add past txt
</commit_message>
<xml_diff>
--- a/NLP/감정별 음악 추천.xlsx
+++ b/NLP/감정별 음악 추천.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="487" uniqueCount="462">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="368">
   <si>
     <t>sad</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1168,69 +1168,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <r>
-      <t>요한</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="돋움"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>파헬벨</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> - </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="돋움"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>캐논</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="돋움"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>변주곡</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>BLACKPINK - Lovesick Girls</t>
   </si>
   <si>
@@ -1418,9 +1355,6 @@
   </si>
   <si>
     <t>태연 - U R</t>
-  </si>
-  <si>
-    <t>태연 - U R</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -1440,9 +1374,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>오마이걸 - Dolphin</t>
-  </si>
-  <si>
     <t>cigarettes after sex - k</t>
   </si>
   <si>
@@ -1753,10 +1684,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Gershwin - Rhapsody in Blue</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>박세아 - 희망 (original version)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1895,9 +1822,6 @@
   </si>
   <si>
     <t>산들 - 취기를 빌려</t>
-  </si>
-  <si>
-    <t>산들 - 취기를 빌려</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -1906,9 +1830,6 @@
   </si>
   <si>
     <t>기리보이 - 연기</t>
-  </si>
-  <si>
-    <t>기리보이 - 연기</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -2009,12 +1930,6 @@
     <t>Bad Blood - Taylor Swift</t>
   </si>
   <si>
-    <t>(여자)아이들 - 덤디덤디</t>
-  </si>
-  <si>
-    <t>Gerda - Burden of Proof</t>
-  </si>
-  <si>
     <t>john legend - never break</t>
   </si>
   <si>
@@ -2027,458 +1942,234 @@
     <t>MAX - Love me less</t>
   </si>
   <si>
-    <t>로꼬 - 잠이들어야</t>
-  </si>
-  <si>
     <t>옥상달빛 - 수고했어, 오늘도</t>
   </si>
   <si>
-    <t>옥상달빛 - 수고했어 오늘도</t>
-  </si>
-  <si>
     <t>엠씨더맥스 - 잠시만안녕</t>
   </si>
   <si>
-    <t>어쿠스틱콜라보 - 응원가</t>
-  </si>
-  <si>
-    <t>휘인 - 헤어지자</t>
-  </si>
-  <si>
-    <t>노래를 안들음</t>
-  </si>
-  <si>
     <t>이효리 - Chitty Chitty Bang Bang</t>
   </si>
   <si>
-    <t>아이유 - 무릎</t>
-  </si>
-  <si>
     <t>Nell - lets take a walk 전곡</t>
   </si>
   <si>
     <t>Walk The Moon - Shup Up and Dance</t>
   </si>
   <si>
-    <t>panic! at the disco - high hopes</t>
-  </si>
-  <si>
     <t>오아시스 - Don't Look Back in Anger</t>
   </si>
   <si>
     <t>자이언티 - 헷갈려</t>
   </si>
   <si>
+    <t>아이유 - 에잇</t>
+  </si>
+  <si>
+    <t>더 크로스 - Don't Cry</t>
+  </si>
+  <si>
+    <t>Andrea Bocelli, Celine Dion- The prayer</t>
+  </si>
+  <si>
+    <t>태연-11:11</t>
+  </si>
+  <si>
+    <t>TONES AND I - DANCE MONKEY</t>
+  </si>
+  <si>
+    <t>식케이 - FIRE</t>
+  </si>
+  <si>
+    <t>죠지 - voat</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>아이유 - unlucky</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>태연 - starlight</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>아이오아이 - When the Cherry Blossom Fade</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>아이유-시간의바깥</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>혁오 - help</t>
+  </si>
+  <si>
+    <t>언니네 이발관 - 아름다운 것</t>
+  </si>
+  <si>
+    <t>Smashing Pumpkins - 1979</t>
+  </si>
+  <si>
+    <t>김동률 - 여름의 끝자락</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>백예린 - rest</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>프라이머리 - 입장정리</t>
+  </si>
+  <si>
+    <t>JazzyFact - 아까워</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>적재 - 나랑 같이 걸을래</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>에픽하이 - 노땡큐</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>엠씨더맥스 - 사계</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>창모- band</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>무키무키만만수 - 안드로메다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2NE1 - Can't Nobody</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>버스커버스커 - 소나기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Simon Dominic - 짠해</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>데이식스 - 좀비</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>블랙핑크 - kill this love</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>블랙핑크 - How you like that</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>트웰브 - Highway</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>마미손 - 별의노래</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>마미손 - 땡큐땡큐</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>매드클라운 - 나쁜 피</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>방탄소년단 - fire</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>빈지노 - break</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>루엘 - Painkiller</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>스윙스, 한요한 - 호루라기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>한요한 - Mood Maker</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>당 디기 방 - 레게 강 같은 평화 RGP</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>한요한 - Baby I'M A ROCKSTAR</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>지코 - 천둥벌거숭이</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>한요한 - 헬리콥터</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>장기하와 얼굴들 - 그렇고 그런 사이</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>Zayde Wolf - Gladiator</t>
-  </si>
-  <si>
-    <t>방탄소년단 - 디오니소스</t>
-  </si>
-  <si>
-    <t>아이유 - 에잇</t>
-  </si>
-  <si>
-    <t>켄-나랑만나볼래요</t>
-  </si>
-  <si>
-    <t>더 크로스 - Don't Cry</t>
-  </si>
-  <si>
-    <t>에픽하이 - 노땡큐</t>
-  </si>
-  <si>
-    <t>안 들음</t>
-  </si>
-  <si>
-    <t>예뻐서 - 유승우</t>
-  </si>
-  <si>
-    <t>사계-mc the max</t>
-  </si>
-  <si>
-    <t>Andrea Bocelli, Celine Dion- The prayer</t>
-  </si>
-  <si>
-    <t>blnk - dead man , 창모- band</t>
-  </si>
-  <si>
-    <t>태연-11:11</t>
-  </si>
-  <si>
-    <t>엑소-love me right, 엑소-call me baby 등 아이돌노래</t>
-  </si>
-  <si>
-    <t>소나기- 버스커버스커// can’t nobody- 2ne1</t>
-  </si>
-  <si>
-    <t>무키무키만만수 - 벌레</t>
-  </si>
-  <si>
-    <t>아이유-무릎</t>
-  </si>
-  <si>
-    <t>태연 - 스트레스</t>
-  </si>
-  <si>
-    <t>개리-또하루 / simon d-짠해 /디오-괜찮아도 괜찮아</t>
-  </si>
-  <si>
-    <t>치즈 - 퇴근시간, 백예린 - 산책</t>
-  </si>
-  <si>
-    <t>환불원정대 - DON'T TOUCH ME</t>
-  </si>
-  <si>
-    <t>Amy Winehouse - Back to Black</t>
-  </si>
-  <si>
-    <t>Gerda - Accusation</t>
-  </si>
-  <si>
-    <t>oasis - stop crying your heart out</t>
-  </si>
-  <si>
-    <t>조용필 - 추억 속의 재회</t>
-  </si>
-  <si>
-    <t>TONES AND I - DANCE MONKEY</t>
-  </si>
-  <si>
-    <t>여행스케치 - 다 잘 될 거야</t>
-  </si>
-  <si>
-    <t>여행스케치 - 산다는건 다 그런게 아니겠니</t>
-  </si>
-  <si>
-    <t>새소년 - 난춘</t>
-  </si>
-  <si>
-    <t>백예린 - Square(2017)</t>
-  </si>
-  <si>
-    <t>빈지노 - break</t>
-  </si>
-  <si>
-    <t>로꼬 - 감아</t>
-  </si>
-  <si>
-    <t>선우정아 - 도망가자</t>
-  </si>
-  <si>
-    <t>CHEEZE - Ticket</t>
-  </si>
-  <si>
-    <t>윤종신 - 지친하루</t>
-  </si>
-  <si>
-    <t>크러쉬 - 어떻게 지내</t>
-  </si>
-  <si>
-    <t>스탠딩 에그 - 무지개</t>
-  </si>
-  <si>
-    <t>멜로망스 - 선물</t>
-  </si>
-  <si>
-    <t>식케이 - FIRE</t>
-  </si>
-  <si>
-    <t>MINO - 몸</t>
-  </si>
-  <si>
-    <t>둘째이모 김다비 - 주라주라</t>
-  </si>
-  <si>
-    <t>지드래곤 - 크래용</t>
-  </si>
-  <si>
-    <t>지오디 - 길</t>
-  </si>
-  <si>
-    <t>아이유 - 이지금</t>
-  </si>
-  <si>
-    <t>Nell - healing process 전곡</t>
-  </si>
-  <si>
-    <t>허각 - 행복한 나를</t>
-  </si>
-  <si>
-    <t>오마이걸 - 꽃차</t>
-  </si>
-  <si>
-    <t>레드벨벳 - 미래</t>
-  </si>
-  <si>
-    <t>The Chainsmokers - Something Just Like This</t>
-  </si>
-  <si>
-    <t>안들음</t>
-  </si>
-  <si>
-    <t>AC/DC - You Shook Me All Night Long</t>
-  </si>
-  <si>
-    <t>매드 클라운 - 나쁜 피</t>
-  </si>
-  <si>
-    <t>청하 - love u</t>
-  </si>
-  <si>
-    <t>The Unlikely Candidates - Oh My Dear Lord</t>
-  </si>
-  <si>
-    <t>The Weeknd - Blinding Lights</t>
-  </si>
-  <si>
-    <t>빈지노 - 브레이크</t>
-  </si>
-  <si>
-    <t>kiiara - gold</t>
-  </si>
-  <si>
-    <t>sg워너비 - 사랑하자</t>
-  </si>
-  <si>
-    <t>방탄소년단 - Filter</t>
-  </si>
-  <si>
-    <t>라붐-상상더하기</t>
-  </si>
-  <si>
-    <t>마마무-HIP</t>
-  </si>
-  <si>
-    <t>더 자두 - 김밥</t>
-  </si>
-  <si>
-    <t>더 넛츠 - 사랑의 바보</t>
-  </si>
-  <si>
-    <t>Dynamite - 방탄소년단</t>
-  </si>
-  <si>
-    <t>최악에 실수와 실수가 반복되는 날</t>
-  </si>
-  <si>
-    <t>예상치 못한 선물이나 금전이 생긴날</t>
-  </si>
-  <si>
-    <t>Painkiller - Ruel</t>
-  </si>
-  <si>
-    <t>사랑한다는 말로는 - 피아노맨</t>
-  </si>
-  <si>
-    <t>방탄 - fire</t>
-  </si>
-  <si>
-    <t>오마이걸 - 돌핀</t>
-  </si>
-  <si>
-    <t>Returns-mc the max</t>
-  </si>
-  <si>
-    <t>Summer hate -지코</t>
-  </si>
-  <si>
-    <t>유튜브 명상음악</t>
-  </si>
-  <si>
-    <t>에버랜드 장미축제 테마곡</t>
-  </si>
-  <si>
-    <t>롤러코스터 - 힘을내요 미스터김</t>
-  </si>
-  <si>
-    <t>펀치 - 영화 속에 나오는 주인공처럼</t>
-  </si>
-  <si>
-    <t>선우정아-도망가자</t>
-  </si>
-  <si>
-    <t>콜드플레이-viva la vida</t>
-  </si>
-  <si>
-    <t>잔잔한 노래, 동물원-시청앞 지하철역에서</t>
-  </si>
-  <si>
-    <t>서프라이즈한 하루가 기억이 나지 않아요. 긍정적으로 서프라이즈한 하루라면 : (여자)아이들-덤디덤디</t>
-  </si>
-  <si>
-    <t>Lonely-종현// 오르막길-윤종신</t>
-  </si>
-  <si>
-    <t>10,000 hours-justin bieber/ tattoos together-lauv</t>
-  </si>
-  <si>
-    <t>윤종신 - 좋니</t>
-  </si>
-  <si>
-    <t>스탠딩에그 - 오래된 노래</t>
-  </si>
-  <si>
-    <t>데이식스-예뻤어</t>
-  </si>
-  <si>
-    <t>Anne-Marie - Trigger</t>
-  </si>
-  <si>
-    <t>아이유-밤편지</t>
-  </si>
-  <si>
-    <t>아이유 - 그 애 참 싫다</t>
-  </si>
-  <si>
-    <t>보아 - 아틀란티스소녀</t>
-  </si>
-  <si>
-    <t>그런날은 노래생각이 안날거같습니다..!</t>
-  </si>
-  <si>
-    <t>아이유-블루밍</t>
-  </si>
-  <si>
-    <t>브로콜리너마저 - 사랑한다는 말로도 위로가 되지 않는, Radiohead - high and dry</t>
-  </si>
-  <si>
-    <t>MGMT - kids, Mariah Carey - all i want for christmas is you</t>
-  </si>
-  <si>
-    <t>bon fire-peder elias</t>
-  </si>
-  <si>
-    <t>wannabe-itzy</t>
-  </si>
-  <si>
-    <t>Coldplay - everglow, 혁오 - Ohio</t>
-  </si>
-  <si>
-    <t>콜드 시</t>
-  </si>
-  <si>
-    <t>오왠 피크닉</t>
-  </si>
-  <si>
-    <t>트와이스 - Feel Special, 동방신기 - Crazy Love, 레드벨벳 - Would U</t>
-  </si>
-  <si>
-    <t>백예린 - Square(2017), 아이유 - Blueming, 알라딘 - A Whole New World</t>
-  </si>
-  <si>
-    <t>적재 - 별보러가자</t>
-  </si>
-  <si>
-    <t>Owl City- Hot Air Balloon</t>
-  </si>
-  <si>
-    <t>사랑은 - 마미손, 나였으면 - 나윤권 등</t>
-  </si>
-  <si>
-    <t>그냥 딱히 ....</t>
-  </si>
-  <si>
-    <t>비욘세 러브온탑</t>
-  </si>
-  <si>
-    <t>오마이걸 돌핀</t>
-  </si>
-  <si>
-    <t>god-길, 볼빨간사춘기-내 사춘기에게, BTS-save me, 화사-maria, 이하이-홀로, 양희은-엄마가 딸에게</t>
-  </si>
-  <si>
-    <t>Imagine dragons-thunder, VERIVERY-Thunder, 방탄소년단-쩔어, 아이유-삐삐, 무한궤도-그대에게</t>
-  </si>
-  <si>
-    <t>엠씨더맥스 - 잠시만 안녕, 린 - 시간을 거슬러</t>
-  </si>
-  <si>
-    <t>B1A4 - 이게 무슨 일이야</t>
-  </si>
-  <si>
-    <t>이소라-신청곡, 종현-lonely</t>
-  </si>
-  <si>
-    <t>Childish gambino - bonfire, Kanye West - POWER</t>
-  </si>
-  <si>
-    <t>위로-권진아</t>
-  </si>
-  <si>
-    <t>블랙핑크 - kill this love, How you like that</t>
-  </si>
-  <si>
-    <t>데이식스 좀비</t>
-  </si>
-  <si>
-    <t>트웰브 - Highway, 서현 - Don't Say No, 휘인 - 내 눈물 모아, 홀스트 - 목성</t>
-  </si>
-  <si>
-    <t>스무살 - 어쩌면 위로가 필요했던 우리</t>
-  </si>
-  <si>
-    <t>이승기-여행을 떠나요, lizzo-juice</t>
-  </si>
-  <si>
-    <t>우효 금요일</t>
-  </si>
-  <si>
-    <t>죠지 - voat</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>아이유 - unlucky</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>태연 - starlight</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>아이오아이 - When the Cherry Blossom Fade</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>아이유-시간의바깥</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>혁오 - help</t>
-  </si>
-  <si>
-    <t>언니네 이발관 - 아름다운 것</t>
-  </si>
-  <si>
-    <t>Smashing Pumpkins - 1979</t>
-  </si>
-  <si>
-    <t>김동률 - 여름의 끝자락</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>백예린 - rest</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>프라이머리 - 입장정리</t>
-  </si>
-  <si>
-    <t>JazzyFact - 아까워</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>남구민 - Reminiscence</t>
-  </si>
-  <si>
-    <t>angry_response</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>horror_response</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>surprise_response</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>grandson - blood</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>The Million - D. M. S</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>renforshort - I drive me mad</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Flor - Imho</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UPSAHL - people I don’t like</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>lola blanc - angry too</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Bishop Briggs - Champion</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Nikki Vianna - Mambo</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>lizzo - juice</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>재즈 음악 모음</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>클래식 음악 모음</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2605,7 +2296,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2634,9 +2325,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -2919,12 +2607,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L82"/>
+  <dimension ref="A1:I82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="H9" sqref="H9"/>
+      <selection pane="bottomLeft" activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -2934,16 +2622,13 @@
     <col min="3" max="3" width="45.3984375" customWidth="1"/>
     <col min="4" max="4" width="53.796875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="43.19921875" customWidth="1"/>
-    <col min="6" max="6" width="8.69921875" customWidth="1"/>
-    <col min="7" max="7" width="29.09765625" customWidth="1"/>
-    <col min="8" max="8" width="111.69921875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="33.796875" customWidth="1"/>
-    <col min="10" max="10" width="29.796875" customWidth="1"/>
-    <col min="11" max="11" width="35.09765625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="74.69921875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.3984375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="111.69921875" customWidth="1"/>
+    <col min="9" max="9" width="74.69921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:7" s="1" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -2965,17 +2650,8 @@
       <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>459</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>460</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>461</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -2989,22 +2665,16 @@
         <v>27</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>298</v>
+        <v>292</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>366</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="I2" t="s">
-        <v>308</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>277</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -3018,22 +2688,10 @@
         <v>29</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>296</v>
-      </c>
-      <c r="G3" t="s">
-        <v>240</v>
-      </c>
-      <c r="I3" t="s">
-        <v>309</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>348</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.3">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -3047,22 +2705,10 @@
         <v>57</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>297</v>
-      </c>
-      <c r="G4" t="s">
-        <v>458</v>
-      </c>
-      <c r="I4" t="s">
-        <v>310</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>350</v>
-      </c>
-      <c r="K4" s="3" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.3">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -3076,19 +2722,10 @@
         <v>72</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>299</v>
-      </c>
-      <c r="I5" t="s">
-        <v>311</v>
-      </c>
-      <c r="J5" s="3" t="s">
-        <v>352</v>
-      </c>
-      <c r="K5" s="3" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -3102,19 +2739,10 @@
         <v>73</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>300</v>
-      </c>
-      <c r="I6" t="s">
-        <v>312</v>
-      </c>
-      <c r="J6" s="3" t="s">
-        <v>353</v>
-      </c>
-      <c r="K6" s="3" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -3128,19 +2756,10 @@
         <v>75</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>301</v>
-      </c>
-      <c r="I7" t="s">
-        <v>313</v>
-      </c>
-      <c r="J7" s="3" t="s">
-        <v>355</v>
-      </c>
-      <c r="K7" s="3" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -3154,19 +2773,10 @@
         <v>74</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>302</v>
-      </c>
-      <c r="I8" t="s">
-        <v>314</v>
-      </c>
-      <c r="J8" s="3" t="s">
-        <v>357</v>
-      </c>
-      <c r="K8" s="3" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -3177,22 +2787,13 @@
         <v>46</v>
       </c>
       <c r="D9" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>303</v>
-      </c>
-      <c r="I9" t="s">
-        <v>315</v>
-      </c>
-      <c r="J9" s="3" t="s">
-        <v>359</v>
-      </c>
-      <c r="K9" s="3" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -3203,22 +2804,13 @@
         <v>76</v>
       </c>
       <c r="D10" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>304</v>
-      </c>
-      <c r="I10" t="s">
-        <v>316</v>
-      </c>
-      <c r="J10" s="3" t="s">
-        <v>361</v>
-      </c>
-      <c r="K10" s="3" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>24</v>
       </c>
@@ -3229,18 +2821,13 @@
         <v>84</v>
       </c>
       <c r="D11" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>306</v>
-      </c>
-      <c r="I11" t="s">
-        <v>317</v>
-      </c>
-      <c r="J11" s="3"/>
-      <c r="K11" s="3"/>
-    </row>
-    <row r="12" spans="1:11" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>25</v>
       </c>
@@ -3251,22 +2838,13 @@
         <v>91</v>
       </c>
       <c r="D12" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>305</v>
-      </c>
-      <c r="I12" t="s">
-        <v>318</v>
-      </c>
-      <c r="J12" s="3" t="s">
-        <v>363</v>
-      </c>
-      <c r="K12" s="3" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>28</v>
       </c>
@@ -3274,25 +2852,16 @@
         <v>78</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="D13" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>307</v>
-      </c>
-      <c r="I13" t="s">
-        <v>319</v>
-      </c>
-      <c r="J13" s="3" t="s">
-        <v>365</v>
-      </c>
-      <c r="K13" s="3" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>33</v>
       </c>
@@ -3300,1286 +2869,1034 @@
         <v>90</v>
       </c>
       <c r="C14" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="D14" t="s">
-        <v>156</v>
-      </c>
-      <c r="E14" s="8"/>
-      <c r="I14" t="s">
-        <v>320</v>
-      </c>
-      <c r="J14" s="3" t="s">
-        <v>320</v>
-      </c>
-      <c r="K14" s="3" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+        <v>153</v>
+      </c>
+      <c r="E14" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>34</v>
       </c>
       <c r="B15" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C15" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="D15" t="s">
-        <v>154</v>
-      </c>
-      <c r="E15" s="8"/>
-      <c r="I15" t="s">
-        <v>321</v>
-      </c>
-      <c r="J15" s="3" t="s">
-        <v>367</v>
-      </c>
-      <c r="K15" s="3" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+        <v>151</v>
+      </c>
+      <c r="E15" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>66</v>
       </c>
       <c r="B16" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C16" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="D16" t="s">
-        <v>248</v>
-      </c>
-      <c r="E16" s="8"/>
-      <c r="I16" t="s">
-        <v>322</v>
-      </c>
-      <c r="J16" s="3" t="s">
-        <v>369</v>
-      </c>
-      <c r="K16" s="3" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+        <v>244</v>
+      </c>
+      <c r="E16" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>35</v>
       </c>
       <c r="B17" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C17" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="D17" t="s">
-        <v>249</v>
-      </c>
-      <c r="E17" s="8"/>
-      <c r="I17" t="s">
-        <v>323</v>
-      </c>
-      <c r="J17" s="3" t="s">
-        <v>371</v>
-      </c>
-      <c r="K17" s="3" t="s">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+        <v>245</v>
+      </c>
+      <c r="E17" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>36</v>
       </c>
       <c r="B18" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C18" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="D18" t="s">
-        <v>157</v>
-      </c>
-      <c r="I18" t="s">
-        <v>324</v>
-      </c>
-      <c r="J18" s="3" t="s">
-        <v>373</v>
-      </c>
-      <c r="K18" s="3" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+        <v>154</v>
+      </c>
+      <c r="E18" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>39</v>
       </c>
       <c r="B19" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C19" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="D19" t="s">
-        <v>158</v>
+        <v>155</v>
+      </c>
+      <c r="E19" t="s">
+        <v>307</v>
       </c>
       <c r="I19" t="s">
-        <v>325</v>
-      </c>
-      <c r="J19" s="10" t="s">
-        <v>375</v>
-      </c>
-      <c r="K19" s="3"/>
-      <c r="L19" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
         <v>38</v>
       </c>
       <c r="B20" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C20" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="D20" t="s">
-        <v>159</v>
-      </c>
-      <c r="I20" t="s">
-        <v>326</v>
-      </c>
-      <c r="J20" s="3" t="s">
-        <v>376</v>
-      </c>
-      <c r="K20" s="3" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+        <v>156</v>
+      </c>
+      <c r="E20" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
         <v>67</v>
       </c>
       <c r="B21" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C21" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="D21" t="s">
-        <v>250</v>
-      </c>
-      <c r="I21" t="s">
-        <v>327</v>
-      </c>
-      <c r="J21" s="3" t="s">
-        <v>378</v>
-      </c>
-      <c r="K21" s="3" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.3">
+        <v>246</v>
+      </c>
+      <c r="E21" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>41</v>
       </c>
       <c r="B22" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C22" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="D22" t="s">
-        <v>251</v>
-      </c>
-      <c r="I22" t="s">
-        <v>328</v>
-      </c>
-      <c r="J22" s="3" t="s">
-        <v>380</v>
-      </c>
-      <c r="K22" s="3" t="s">
-        <v>381</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+        <v>247</v>
+      </c>
+      <c r="E22" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>42</v>
       </c>
       <c r="B23" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C23" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="D23" t="s">
-        <v>160</v>
-      </c>
-      <c r="I23" t="s">
-        <v>329</v>
-      </c>
-      <c r="J23" s="3" t="s">
-        <v>382</v>
-      </c>
-      <c r="K23" s="3" t="s">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+        <v>157</v>
+      </c>
+      <c r="E23" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B24" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C24" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="D24" t="s">
-        <v>166</v>
-      </c>
-      <c r="I24" t="s">
-        <v>330</v>
-      </c>
-      <c r="J24" s="3" t="s">
-        <v>384</v>
-      </c>
-      <c r="K24" s="3" t="s">
-        <v>385</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+        <v>163</v>
+      </c>
+      <c r="E24" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>44</v>
       </c>
       <c r="B25" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C25" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="D25" t="s">
-        <v>252</v>
-      </c>
-      <c r="I25" t="s">
-        <v>331</v>
-      </c>
-      <c r="J25" s="3" t="s">
-        <v>386</v>
-      </c>
-      <c r="K25" s="3" t="s">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+        <v>248</v>
+      </c>
+      <c r="E25" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>45</v>
       </c>
       <c r="B26" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C26" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="D26" t="s">
-        <v>161</v>
-      </c>
-      <c r="I26" t="s">
-        <v>332</v>
-      </c>
-      <c r="J26" s="3" t="s">
-        <v>388</v>
-      </c>
-      <c r="K26" s="3" t="s">
-        <v>389</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+        <v>158</v>
+      </c>
+      <c r="E26" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>47</v>
       </c>
       <c r="B27" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C27" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="D27" t="s">
-        <v>162</v>
-      </c>
-      <c r="I27" t="s">
-        <v>333</v>
-      </c>
-      <c r="J27" s="3" t="s">
-        <v>280</v>
-      </c>
-      <c r="K27" s="3" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+        <v>159</v>
+      </c>
+      <c r="E27" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
         <v>48</v>
       </c>
       <c r="B28" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C28" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="D28" t="s">
-        <v>163</v>
-      </c>
-      <c r="J28" s="3" t="s">
-        <v>334</v>
-      </c>
-      <c r="K28" s="3" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.3">
+        <v>160</v>
+      </c>
+      <c r="E28" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
         <v>49</v>
       </c>
       <c r="B29" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C29" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="D29" t="s">
-        <v>164</v>
-      </c>
-      <c r="J29" s="3" t="s">
-        <v>391</v>
-      </c>
-      <c r="K29" s="3" t="s">
-        <v>392</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+        <v>161</v>
+      </c>
+      <c r="E29" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
         <v>52</v>
       </c>
       <c r="B30" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C30" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D30" t="s">
-        <v>254</v>
-      </c>
-      <c r="I30" t="s">
-        <v>335</v>
-      </c>
-      <c r="J30" s="3" t="s">
-        <v>393</v>
-      </c>
-      <c r="K30" s="3" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+        <v>250</v>
+      </c>
+      <c r="E30" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>51</v>
       </c>
       <c r="B31" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C31" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="D31" t="s">
-        <v>255</v>
-      </c>
-      <c r="I31" t="s">
-        <v>315</v>
-      </c>
-      <c r="J31" s="3" t="s">
-        <v>395</v>
-      </c>
-      <c r="K31" s="3" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+        <v>251</v>
+      </c>
+      <c r="E31" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
         <v>54</v>
       </c>
       <c r="B32" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C32" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="D32" t="s">
-        <v>256</v>
-      </c>
-      <c r="I32" t="s">
-        <v>336</v>
-      </c>
-      <c r="J32" s="3" t="s">
-        <v>397</v>
-      </c>
-      <c r="K32" s="3" t="s">
-        <v>398</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+        <v>252</v>
+      </c>
+      <c r="E32" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>55</v>
       </c>
       <c r="B33" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C33" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="D33" t="s">
-        <v>257</v>
-      </c>
-      <c r="I33" t="s">
-        <v>337</v>
-      </c>
-      <c r="J33" s="3" t="s">
-        <v>399</v>
-      </c>
-      <c r="K33" s="3" t="s">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11" ht="28.2" thickBot="1" x14ac:dyDescent="0.4">
+        <v>253</v>
+      </c>
+      <c r="E33" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A34" s="4" t="s">
         <v>68</v>
       </c>
       <c r="B34" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C34" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="D34" t="s">
-        <v>258</v>
-      </c>
-      <c r="I34" t="s">
-        <v>338</v>
-      </c>
-      <c r="J34" s="3" t="s">
-        <v>401</v>
-      </c>
-      <c r="K34" s="3" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+        <v>254</v>
+      </c>
+      <c r="E34" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="s">
         <v>69</v>
       </c>
       <c r="B35" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C35" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="D35" t="s">
-        <v>259</v>
-      </c>
-      <c r="I35" t="s">
-        <v>339</v>
-      </c>
-      <c r="J35" s="3" t="s">
-        <v>403</v>
-      </c>
-      <c r="K35" s="3" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.3">
+        <v>255</v>
+      </c>
+      <c r="E35" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
         <v>58</v>
       </c>
       <c r="B36" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C36" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="D36" t="s">
-        <v>260</v>
-      </c>
-      <c r="I36" t="s">
-        <v>340</v>
-      </c>
-      <c r="J36" s="3" t="s">
-        <v>405</v>
-      </c>
-      <c r="K36" s="3" t="s">
-        <v>406</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+        <v>256</v>
+      </c>
+      <c r="E36" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
         <v>71</v>
       </c>
       <c r="B37" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C37" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="D37" t="s">
-        <v>261</v>
-      </c>
-      <c r="I37" t="s">
-        <v>341</v>
-      </c>
-      <c r="J37" s="3" t="s">
-        <v>407</v>
-      </c>
-      <c r="K37" s="3" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+        <v>257</v>
+      </c>
+      <c r="E37" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="3" t="s">
         <v>59</v>
       </c>
       <c r="B38" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C38" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="D38" t="s">
-        <v>262</v>
-      </c>
-      <c r="I38" t="s">
-        <v>342</v>
-      </c>
-      <c r="J38" s="3" t="s">
-        <v>409</v>
-      </c>
-      <c r="K38" s="3" t="s">
-        <v>410</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+        <v>258</v>
+      </c>
+      <c r="E38" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
         <v>60</v>
       </c>
       <c r="B39" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C39" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="D39" t="s">
-        <v>263</v>
-      </c>
-      <c r="I39" t="s">
-        <v>343</v>
-      </c>
-      <c r="J39" s="3" t="s">
-        <v>343</v>
-      </c>
-      <c r="K39" s="3" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="40" spans="1:11" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+        <v>259</v>
+      </c>
+      <c r="E39" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
         <v>61</v>
       </c>
       <c r="B40" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C40" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="D40" t="s">
-        <v>264</v>
-      </c>
-      <c r="I40" t="s">
-        <v>344</v>
-      </c>
-      <c r="J40" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="K40" s="3" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="41" spans="1:11" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+        <v>260</v>
+      </c>
+      <c r="E40" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
         <v>63</v>
       </c>
       <c r="B41" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C41" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="D41" t="s">
-        <v>265</v>
-      </c>
-      <c r="I41" t="s">
-        <v>345</v>
-      </c>
-      <c r="J41" s="3" t="s">
-        <v>413</v>
-      </c>
-      <c r="K41" s="3"/>
-    </row>
-    <row r="42" spans="1:11" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+        <v>261</v>
+      </c>
+      <c r="E41" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
         <v>50</v>
       </c>
       <c r="B42" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C42" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="D42" t="s">
-        <v>266</v>
-      </c>
-      <c r="I42" t="s">
-        <v>346</v>
-      </c>
-      <c r="J42" s="3" t="s">
-        <v>414</v>
-      </c>
-      <c r="K42" s="3" t="s">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="43" spans="1:11" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+        <v>262</v>
+      </c>
+      <c r="E42" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
         <v>77</v>
       </c>
       <c r="B43" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C43" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="D43" t="s">
-        <v>168</v>
-      </c>
-      <c r="J43" s="3"/>
-      <c r="K43" s="3"/>
-    </row>
-    <row r="44" spans="1:11" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.3">
+        <v>165</v>
+      </c>
+      <c r="E43" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
         <v>64</v>
       </c>
       <c r="B44" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C44" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="D44" t="s">
-        <v>267</v>
-      </c>
-      <c r="J44" s="3" t="s">
-        <v>416</v>
-      </c>
-      <c r="K44" s="3" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="45" spans="1:11" ht="79.8" thickBot="1" x14ac:dyDescent="0.3">
+        <v>263</v>
+      </c>
+      <c r="E44" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
         <v>79</v>
       </c>
       <c r="B45" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C45" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="D45" t="s">
-        <v>268</v>
-      </c>
-      <c r="J45" s="3" t="s">
-        <v>418</v>
-      </c>
-      <c r="K45" s="3" t="s">
-        <v>419</v>
-      </c>
-    </row>
-    <row r="46" spans="1:11" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+        <v>264</v>
+      </c>
+      <c r="E45" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>80</v>
       </c>
       <c r="B46" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C46" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="D46" t="s">
-        <v>270</v>
-      </c>
-      <c r="J46" s="3" t="s">
-        <v>420</v>
-      </c>
-      <c r="K46" s="3" t="s">
-        <v>421</v>
-      </c>
-    </row>
-    <row r="47" spans="1:11" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.3">
+        <v>266</v>
+      </c>
+      <c r="E46" s="3" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>81</v>
       </c>
       <c r="B47" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C47" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="D47" t="s">
-        <v>269</v>
-      </c>
-      <c r="J47" s="3" t="s">
-        <v>422</v>
-      </c>
-      <c r="K47" s="3" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="48" spans="1:11" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+        <v>265</v>
+      </c>
+      <c r="E47" s="3" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A48" t="s">
         <v>82</v>
       </c>
       <c r="B48" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C48" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="D48" t="s">
-        <v>271</v>
-      </c>
-      <c r="J48" s="3" t="s">
-        <v>423</v>
-      </c>
-      <c r="K48" s="3" t="s">
-        <v>424</v>
-      </c>
-    </row>
-    <row r="49" spans="1:11" ht="66.599999999999994" thickBot="1" x14ac:dyDescent="0.3">
+        <v>267</v>
+      </c>
+      <c r="E48" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
         <v>65</v>
       </c>
       <c r="B49" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C49" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="D49" t="s">
-        <v>272</v>
-      </c>
-      <c r="J49" s="3" t="s">
-        <v>425</v>
-      </c>
-      <c r="K49" s="3" t="s">
-        <v>426</v>
-      </c>
-    </row>
-    <row r="50" spans="1:11" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+        <v>268</v>
+      </c>
+      <c r="E49" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A50" t="s">
         <v>83</v>
       </c>
       <c r="B50" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C50" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="D50" t="s">
-        <v>273</v>
-      </c>
-      <c r="J50" s="3" t="s">
-        <v>427</v>
-      </c>
-      <c r="K50" s="3" t="s">
-        <v>428</v>
-      </c>
-    </row>
-    <row r="51" spans="1:11" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.3">
+        <v>269</v>
+      </c>
+      <c r="E50" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A51" t="s">
         <v>85</v>
       </c>
       <c r="B51" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C51" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="D51" t="s">
-        <v>274</v>
-      </c>
-      <c r="J51" s="3" t="s">
-        <v>429</v>
-      </c>
-      <c r="K51" s="3" t="s">
-        <v>430</v>
-      </c>
-    </row>
-    <row r="52" spans="1:11" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+        <v>270</v>
+      </c>
+      <c r="E51" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A52" t="s">
         <v>87</v>
       </c>
       <c r="B52" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C52" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="D52" t="s">
-        <v>275</v>
-      </c>
-      <c r="J52" s="3" t="s">
-        <v>431</v>
-      </c>
-      <c r="K52" s="3" t="s">
-        <v>432</v>
-      </c>
-    </row>
-    <row r="53" spans="1:11" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+        <v>271</v>
+      </c>
+      <c r="E52" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A53" t="s">
         <v>88</v>
       </c>
       <c r="B53" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C53" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="D53" t="s">
-        <v>276</v>
-      </c>
-      <c r="J53" s="3"/>
-      <c r="K53" s="3"/>
-    </row>
-    <row r="54" spans="1:11" ht="93" thickBot="1" x14ac:dyDescent="0.3">
+        <v>272</v>
+      </c>
+      <c r="E53" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
         <v>86</v>
       </c>
       <c r="B54" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C54" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="D54" t="s">
-        <v>279</v>
-      </c>
-      <c r="J54" s="3" t="s">
-        <v>433</v>
-      </c>
-      <c r="K54" s="3" t="s">
-        <v>434</v>
-      </c>
-    </row>
-    <row r="55" spans="1:11" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+        <v>274</v>
+      </c>
+      <c r="E54" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A55" t="s">
         <v>89</v>
       </c>
       <c r="B55" t="s">
+        <v>139</v>
+      </c>
+      <c r="C55" t="s">
+        <v>220</v>
+      </c>
+      <c r="D55" t="s">
+        <v>275</v>
+      </c>
+      <c r="E55" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A56" t="s">
+        <v>150</v>
+      </c>
+      <c r="B56" t="s">
         <v>140</v>
       </c>
-      <c r="C55" t="s">
+      <c r="C56" t="s">
+        <v>221</v>
+      </c>
+      <c r="D56" t="s">
+        <v>276</v>
+      </c>
+      <c r="E56" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A57" t="s">
+        <v>168</v>
+      </c>
+      <c r="B57" t="s">
+        <v>141</v>
+      </c>
+      <c r="C57" t="s">
+        <v>222</v>
+      </c>
+      <c r="D57" t="s">
+        <v>278</v>
+      </c>
+      <c r="E57" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A58" t="s">
+        <v>273</v>
+      </c>
+      <c r="B58" t="s">
+        <v>110</v>
+      </c>
+      <c r="C58" t="s">
         <v>223</v>
       </c>
-      <c r="D55" t="s">
+      <c r="D58" t="s">
+        <v>279</v>
+      </c>
+      <c r="E58" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A59" t="s">
+        <v>331</v>
+      </c>
+      <c r="B59" t="s">
+        <v>108</v>
+      </c>
+      <c r="C59" t="s">
+        <v>210</v>
+      </c>
+      <c r="D59" t="s">
+        <v>280</v>
+      </c>
+      <c r="E59" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="B60" t="s">
+        <v>143</v>
+      </c>
+      <c r="C60" t="s">
+        <v>225</v>
+      </c>
+      <c r="D60" t="s">
+        <v>283</v>
+      </c>
+      <c r="E60" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="B61" t="s">
+        <v>142</v>
+      </c>
+      <c r="C61" t="s">
+        <v>226</v>
+      </c>
+      <c r="D61" t="s">
+        <v>284</v>
+      </c>
+      <c r="E61" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="B62" t="s">
+        <v>144</v>
+      </c>
+      <c r="C62" t="s">
+        <v>166</v>
+      </c>
+      <c r="D62" t="s">
+        <v>285</v>
+      </c>
+      <c r="E62" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="B63" t="s">
+        <v>145</v>
+      </c>
+      <c r="C63" t="s">
+        <v>169</v>
+      </c>
+      <c r="D63" t="s">
+        <v>286</v>
+      </c>
+      <c r="E63" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="B64" t="s">
+        <v>147</v>
+      </c>
+      <c r="C64" t="s">
+        <v>228</v>
+      </c>
+      <c r="D64" t="s">
+        <v>287</v>
+      </c>
+      <c r="E64" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="65" spans="2:4" x14ac:dyDescent="0.4">
+      <c r="B65" t="s">
+        <v>146</v>
+      </c>
+      <c r="C65" t="s">
+        <v>229</v>
+      </c>
+      <c r="D65" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="66" spans="2:4" x14ac:dyDescent="0.4">
+      <c r="B66" t="s">
+        <v>112</v>
+      </c>
+      <c r="C66" t="s">
+        <v>224</v>
+      </c>
+      <c r="D66" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="67" spans="2:4" x14ac:dyDescent="0.4">
+      <c r="B67" t="s">
+        <v>113</v>
+      </c>
+      <c r="C67" t="s">
+        <v>230</v>
+      </c>
+      <c r="D67" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="68" spans="2:4" x14ac:dyDescent="0.4">
+      <c r="B68" t="s">
+        <v>148</v>
+      </c>
+      <c r="C68" t="s">
+        <v>231</v>
+      </c>
+      <c r="D68" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="69" spans="2:4" x14ac:dyDescent="0.4">
+      <c r="B69" t="s">
+        <v>149</v>
+      </c>
+      <c r="C69" t="s">
+        <v>232</v>
+      </c>
+      <c r="D69" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="70" spans="2:4" x14ac:dyDescent="0.4">
+      <c r="B70" t="s">
+        <v>182</v>
+      </c>
+      <c r="C70" t="s">
+        <v>233</v>
+      </c>
+      <c r="D70" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="71" spans="2:4" x14ac:dyDescent="0.4">
+      <c r="B71" t="s">
+        <v>187</v>
+      </c>
+      <c r="C71" t="s">
+        <v>234</v>
+      </c>
+      <c r="D71" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="72" spans="2:4" x14ac:dyDescent="0.4">
+      <c r="B72" t="s">
+        <v>204</v>
+      </c>
+      <c r="C72" t="s">
+        <v>235</v>
+      </c>
+      <c r="D72" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="73" spans="2:4" x14ac:dyDescent="0.4">
+      <c r="B73" t="s">
+        <v>206</v>
+      </c>
+      <c r="C73" t="s">
+        <v>236</v>
+      </c>
+      <c r="D73" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="74" spans="2:4" x14ac:dyDescent="0.4">
+      <c r="B74" t="s">
+        <v>207</v>
+      </c>
+      <c r="C74" t="s">
+        <v>237</v>
+      </c>
+      <c r="D74" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="75" spans="2:4" x14ac:dyDescent="0.4">
+      <c r="B75" t="s">
+        <v>180</v>
+      </c>
+      <c r="C75" t="s">
+        <v>178</v>
+      </c>
+      <c r="D75" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="76" spans="2:4" x14ac:dyDescent="0.4">
+      <c r="B76" t="s">
+        <v>209</v>
+      </c>
+      <c r="C76" t="s">
+        <v>238</v>
+      </c>
+      <c r="D76" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="77" spans="2:4" x14ac:dyDescent="0.4">
+      <c r="B77" t="s">
+        <v>208</v>
+      </c>
+      <c r="C77" t="s">
+        <v>239</v>
+      </c>
+      <c r="D77" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="78" spans="2:4" x14ac:dyDescent="0.4">
+      <c r="B78" t="s">
+        <v>162</v>
+      </c>
+      <c r="C78" t="s">
+        <v>240</v>
+      </c>
+      <c r="D78" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="79" spans="2:4" x14ac:dyDescent="0.4">
+      <c r="B79" t="s">
+        <v>277</v>
+      </c>
+      <c r="C79" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="80" spans="2:4" x14ac:dyDescent="0.4">
+      <c r="B80" t="s">
         <v>281</v>
       </c>
-      <c r="J55" s="3"/>
-      <c r="K55" s="3"/>
-    </row>
-    <row r="56" spans="1:11" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A56" t="s">
+      <c r="C80" t="s">
         <v>152</v>
-      </c>
-      <c r="B56" t="s">
-        <v>141</v>
-      </c>
-      <c r="C56" t="s">
-        <v>224</v>
-      </c>
-      <c r="D56" t="s">
-        <v>282</v>
-      </c>
-      <c r="J56" s="3" t="s">
-        <v>435</v>
-      </c>
-      <c r="K56" s="3" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A57" t="s">
-        <v>171</v>
-      </c>
-      <c r="B57" t="s">
-        <v>142</v>
-      </c>
-      <c r="C57" t="s">
-        <v>225</v>
-      </c>
-      <c r="D57" t="s">
-        <v>284</v>
-      </c>
-      <c r="I57" t="s">
-        <v>437</v>
-      </c>
-      <c r="J57" t="s">
-        <v>416</v>
-      </c>
-      <c r="K57" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A58" t="s">
-        <v>278</v>
-      </c>
-      <c r="B58" t="s">
-        <v>111</v>
-      </c>
-      <c r="C58" t="s">
-        <v>226</v>
-      </c>
-      <c r="D58" t="s">
-        <v>285</v>
-      </c>
-      <c r="I58" t="s">
-        <v>438</v>
-      </c>
-      <c r="J58" t="s">
-        <v>418</v>
-      </c>
-      <c r="K58" t="s">
-        <v>419</v>
-      </c>
-    </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="B59" t="s">
-        <v>109</v>
-      </c>
-      <c r="C59" t="s">
-        <v>213</v>
-      </c>
-      <c r="D59" t="s">
-        <v>286</v>
-      </c>
-      <c r="I59" t="s">
-        <v>439</v>
-      </c>
-      <c r="J59" t="s">
-        <v>420</v>
-      </c>
-      <c r="K59" t="s">
-        <v>421</v>
-      </c>
-    </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="B60" t="s">
-        <v>144</v>
-      </c>
-      <c r="C60" t="s">
-        <v>228</v>
-      </c>
-      <c r="D60" t="s">
-        <v>289</v>
-      </c>
-      <c r="I60" t="s">
-        <v>440</v>
-      </c>
-      <c r="J60" t="s">
-        <v>422</v>
-      </c>
-      <c r="K60" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="B61" t="s">
-        <v>143</v>
-      </c>
-      <c r="C61" t="s">
-        <v>229</v>
-      </c>
-      <c r="D61" t="s">
-        <v>290</v>
-      </c>
-      <c r="I61" t="s">
-        <v>441</v>
-      </c>
-      <c r="J61" t="s">
-        <v>423</v>
-      </c>
-      <c r="K61" t="s">
-        <v>424</v>
-      </c>
-    </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="B62" t="s">
-        <v>145</v>
-      </c>
-      <c r="C62" t="s">
-        <v>169</v>
-      </c>
-      <c r="D62" t="s">
-        <v>291</v>
-      </c>
-      <c r="I62" t="s">
-        <v>442</v>
-      </c>
-      <c r="J62" t="s">
-        <v>425</v>
-      </c>
-      <c r="K62" t="s">
-        <v>426</v>
-      </c>
-    </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="B63" t="s">
-        <v>146</v>
-      </c>
-      <c r="C63" t="s">
-        <v>172</v>
-      </c>
-      <c r="D63" t="s">
-        <v>292</v>
-      </c>
-      <c r="I63" t="s">
-        <v>443</v>
-      </c>
-      <c r="J63" t="s">
-        <v>427</v>
-      </c>
-      <c r="K63" t="s">
-        <v>428</v>
-      </c>
-    </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="B64" t="s">
-        <v>149</v>
-      </c>
-      <c r="C64" t="s">
-        <v>231</v>
-      </c>
-      <c r="D64" t="s">
-        <v>293</v>
-      </c>
-      <c r="I64" t="s">
-        <v>444</v>
-      </c>
-      <c r="J64" t="s">
-        <v>429</v>
-      </c>
-      <c r="K64" t="s">
-        <v>430</v>
-      </c>
-    </row>
-    <row r="65" spans="2:11" x14ac:dyDescent="0.4">
-      <c r="B65" t="s">
-        <v>148</v>
-      </c>
-      <c r="C65" t="s">
-        <v>232</v>
-      </c>
-      <c r="D65" t="s">
-        <v>294</v>
-      </c>
-      <c r="I65" t="s">
-        <v>445</v>
-      </c>
-      <c r="J65" t="s">
-        <v>431</v>
-      </c>
-      <c r="K65" t="s">
-        <v>432</v>
-      </c>
-    </row>
-    <row r="66" spans="2:11" x14ac:dyDescent="0.4">
-      <c r="B66" t="s">
-        <v>113</v>
-      </c>
-      <c r="C66" t="s">
-        <v>227</v>
-      </c>
-      <c r="D66" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="67" spans="2:11" x14ac:dyDescent="0.4">
-      <c r="B67" t="s">
-        <v>114</v>
-      </c>
-      <c r="C67" t="s">
-        <v>233</v>
-      </c>
-      <c r="D67" t="s">
-        <v>446</v>
-      </c>
-    </row>
-    <row r="68" spans="2:11" x14ac:dyDescent="0.4">
-      <c r="B68" t="s">
-        <v>150</v>
-      </c>
-      <c r="C68" t="s">
-        <v>234</v>
-      </c>
-      <c r="D68" t="s">
-        <v>448</v>
-      </c>
-    </row>
-    <row r="69" spans="2:11" x14ac:dyDescent="0.4">
-      <c r="B69" t="s">
-        <v>151</v>
-      </c>
-      <c r="C69" t="s">
-        <v>235</v>
-      </c>
-      <c r="D69" t="s">
-        <v>449</v>
-      </c>
-    </row>
-    <row r="70" spans="2:11" x14ac:dyDescent="0.4">
-      <c r="B70" t="s">
-        <v>185</v>
-      </c>
-      <c r="C70" t="s">
-        <v>236</v>
-      </c>
-      <c r="D70" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="71" spans="2:11" x14ac:dyDescent="0.4">
-      <c r="B71" t="s">
-        <v>190</v>
-      </c>
-      <c r="C71" t="s">
-        <v>237</v>
-      </c>
-      <c r="D71" t="s">
-        <v>447</v>
-      </c>
-    </row>
-    <row r="72" spans="2:11" x14ac:dyDescent="0.4">
-      <c r="B72" t="s">
-        <v>207</v>
-      </c>
-      <c r="C72" t="s">
-        <v>238</v>
-      </c>
-      <c r="D72" t="s">
-        <v>451</v>
-      </c>
-    </row>
-    <row r="73" spans="2:11" x14ac:dyDescent="0.4">
-      <c r="B73" t="s">
-        <v>209</v>
-      </c>
-      <c r="C73" t="s">
-        <v>239</v>
-      </c>
-      <c r="D73" t="s">
-        <v>452</v>
-      </c>
-    </row>
-    <row r="74" spans="2:11" x14ac:dyDescent="0.4">
-      <c r="B74" t="s">
-        <v>210</v>
-      </c>
-      <c r="C74" t="s">
-        <v>241</v>
-      </c>
-      <c r="D74" t="s">
-        <v>453</v>
-      </c>
-    </row>
-    <row r="75" spans="2:11" x14ac:dyDescent="0.4">
-      <c r="B75" t="s">
-        <v>183</v>
-      </c>
-      <c r="C75" t="s">
-        <v>181</v>
-      </c>
-      <c r="D75" t="s">
-        <v>454</v>
-      </c>
-    </row>
-    <row r="76" spans="2:11" x14ac:dyDescent="0.4">
-      <c r="B76" t="s">
-        <v>212</v>
-      </c>
-      <c r="C76" t="s">
-        <v>242</v>
-      </c>
-      <c r="D76" t="s">
-        <v>455</v>
-      </c>
-    </row>
-    <row r="77" spans="2:11" x14ac:dyDescent="0.4">
-      <c r="B77" t="s">
-        <v>211</v>
-      </c>
-      <c r="C77" t="s">
-        <v>243</v>
-      </c>
-      <c r="D77" t="s">
-        <v>456</v>
-      </c>
-    </row>
-    <row r="78" spans="2:11" x14ac:dyDescent="0.4">
-      <c r="B78" t="s">
-        <v>165</v>
-      </c>
-      <c r="C78" t="s">
-        <v>244</v>
-      </c>
-      <c r="D78" t="s">
-        <v>457</v>
-      </c>
-    </row>
-    <row r="79" spans="2:11" x14ac:dyDescent="0.4">
-      <c r="B79" t="s">
-        <v>283</v>
-      </c>
-      <c r="C79" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="80" spans="2:11" x14ac:dyDescent="0.4">
-      <c r="B80" t="s">
-        <v>287</v>
-      </c>
-      <c r="C80" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="81" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B81" t="s">
-        <v>288</v>
+        <v>282</v>
       </c>
       <c r="C81" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
     </row>
     <row r="82" spans="2:3" x14ac:dyDescent="0.4">
       <c r="C82" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
     </row>
   </sheetData>

</xml_diff>